<commit_message>
adicionado local/data/hora em criarEvento
</commit_message>
<xml_diff>
--- a/Documentação/PRODUT_BACKLOG 1 (1).xlsx
+++ b/Documentação/PRODUT_BACKLOG 1 (1).xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John_Ortsac\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF8008DC-8329-4EF1-96AD-155D7FDCC3BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16608" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +30,6 @@
     <t>PRODUT BACKLOG DO PRIMEIRO MÓDULO</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1 - Criar uma pagina para cadastro e log in do administrador: Nesta pagina terá duas opções que serão redirecionadas para pagina de log in ou para a pagina de cadastro.</t>
-  </si>
-  <si>
     <t>2 - Criar uma pagina para a criação do evento.</t>
   </si>
   <si>
@@ -69,12 +60,15 @@
   <si>
     <t>10 - Ao compartilhar o evento nas redes sociais será criado um código que funcionará como cupom de desconto para atividades pagas.</t>
   </si>
+  <si>
+    <t xml:space="preserve"> 1 - Criar uma pagina para cadastro e login do administrador:Nesta pagina terá duas opções que serão redirecionadas para pagina de log in ou para a pagina de cadastro.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,96 +413,96 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="31.5" customHeight="1">
+    <row r="1" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="2:6" ht="50.25" customHeight="1">
+    <row r="2" spans="2:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="2:6" ht="45" customHeight="1">
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="2:6" ht="31.5" customHeight="1">
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="2:6" ht="21" customHeight="1">
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="2:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="2:6" ht="105.75" customHeight="1">
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="2:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="2:6" ht="90.75" customHeight="1">
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="2:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="2:6" ht="60.75" customHeight="1">
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="2:6" ht="21" customHeight="1">
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="2:6" ht="31.5">
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="2:6" ht="31.5">
-      <c r="B11" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="C11" s="6"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="23" spans="4:4" ht="15.75">
+    <row r="23" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D23" s="3"/>
     </row>
   </sheetData>

</xml_diff>